<commit_message>
Update 00. PARTS LIST.xlsx, AMS1117x.x.pdf, and HD74LS73AP.pdf
</commit_message>
<xml_diff>
--- a/00. PARTS LIST.xlsx
+++ b/00. PARTS LIST.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PROCESSOR\Desktop\Justin\datasheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin\Documents\workspace\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA56B43-09A3-41D9-9952-8B26CC567B02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3600" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="4050" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$K$315</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$K$318</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="914">
   <si>
     <t>IC CHIP / PARTS LIST</t>
   </si>
@@ -3092,13 +3093,44 @@
   </si>
   <si>
     <t>B07-07</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HD74LS73AP</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>A16-01</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flip-Flop</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FILE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dual J-K Flip-Flops (with Preset, Common Clear, and Common Clock)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>OSCILLATOR</t>
+  </si>
+  <si>
+    <t>MODULE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Voltage Regulator</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월 &quot;dd&quot;일&quot;"/>
   </numFmts>
@@ -3195,7 +3227,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3250,9 +3282,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Text 1" xfId="2"/>
+    <cellStyle name="Text 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
@@ -3599,12 +3634,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ1217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K94" sqref="K94"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A311" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G322" sqref="G322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -3614,7 +3649,7 @@
     <col min="3" max="4" width="8.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="73.875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="77.5" style="5" customWidth="1"/>
     <col min="8" max="8" width="6.25" style="4" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" style="4" customWidth="1"/>
@@ -9235,7 +9270,10 @@
       </c>
       <c r="G288" s="6"/>
     </row>
-    <row r="289" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A289" s="4">
+        <v>286</v>
+      </c>
       <c r="B289" s="1" t="s">
         <v>830</v>
       </c>
@@ -9250,7 +9288,10 @@
       </c>
       <c r="G289" s="6"/>
     </row>
-    <row r="290" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A290" s="4">
+        <v>287</v>
+      </c>
       <c r="B290" s="1" t="s">
         <v>833</v>
       </c>
@@ -9265,106 +9306,181 @@
       </c>
       <c r="G290" s="6"/>
     </row>
-    <row r="291" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A291" s="4">
+        <v>288</v>
+      </c>
       <c r="B291" s="1" t="s">
         <v>834</v>
       </c>
       <c r="C291" s="1" t="s">
         <v>836</v>
       </c>
+      <c r="F291" s="1" t="s">
+        <v>913</v>
+      </c>
       <c r="G291" s="6"/>
-    </row>
-    <row r="292" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="J291" s="18" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A292" s="4">
+        <v>289</v>
+      </c>
       <c r="B292" s="1" t="s">
         <v>835</v>
       </c>
       <c r="C292" s="1" t="s">
         <v>837</v>
       </c>
+      <c r="F292" s="1" t="s">
+        <v>913</v>
+      </c>
       <c r="G292" s="6"/>
-    </row>
-    <row r="293" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="J292" s="18" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A293" s="4">
+        <v>290</v>
+      </c>
       <c r="B293" s="1" t="s">
         <v>838</v>
       </c>
       <c r="C293" s="1" t="s">
         <v>839</v>
       </c>
+      <c r="F293" s="1" t="s">
+        <v>911</v>
+      </c>
       <c r="G293" s="6"/>
     </row>
-    <row r="294" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A294" s="4">
+        <v>291</v>
+      </c>
       <c r="B294" s="1" t="s">
         <v>852</v>
       </c>
       <c r="C294" s="1" t="s">
         <v>840</v>
       </c>
+      <c r="F294" s="1" t="s">
+        <v>911</v>
+      </c>
       <c r="G294" s="6"/>
     </row>
-    <row r="295" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A295" s="4">
+        <v>292</v>
+      </c>
       <c r="B295" s="1" t="s">
         <v>853</v>
       </c>
       <c r="C295" s="1" t="s">
         <v>841</v>
       </c>
+      <c r="F295" s="1" t="s">
+        <v>911</v>
+      </c>
       <c r="G295" s="6"/>
     </row>
-    <row r="296" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A296" s="4">
+        <v>293</v>
+      </c>
       <c r="B296" s="1" t="s">
         <v>854</v>
       </c>
       <c r="C296" s="1" t="s">
         <v>842</v>
       </c>
+      <c r="F296" s="1" t="s">
+        <v>911</v>
+      </c>
       <c r="G296" s="6"/>
     </row>
-    <row r="297" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A297" s="4">
+        <v>294</v>
+      </c>
       <c r="B297" s="1" t="s">
         <v>855</v>
       </c>
       <c r="C297" s="1" t="s">
         <v>843</v>
       </c>
+      <c r="F297" s="1" t="s">
+        <v>912</v>
+      </c>
       <c r="G297" s="6"/>
     </row>
-    <row r="298" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A298" s="4">
+        <v>295</v>
+      </c>
       <c r="B298" s="1" t="s">
         <v>856</v>
       </c>
       <c r="C298" s="1" t="s">
         <v>844</v>
       </c>
+      <c r="F298" s="1" t="s">
+        <v>911</v>
+      </c>
       <c r="G298" s="6"/>
     </row>
-    <row r="299" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A299" s="4">
+        <v>296</v>
+      </c>
       <c r="B299" s="1" t="s">
         <v>857</v>
       </c>
       <c r="C299" s="1" t="s">
         <v>845</v>
       </c>
+      <c r="F299" s="1" t="s">
+        <v>911</v>
+      </c>
       <c r="G299" s="6"/>
     </row>
-    <row r="300" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A300" s="4">
+        <v>297</v>
+      </c>
       <c r="B300" s="1" t="s">
         <v>858</v>
       </c>
       <c r="C300" s="1" t="s">
         <v>846</v>
       </c>
+      <c r="F300" s="1" t="s">
+        <v>911</v>
+      </c>
       <c r="G300" s="6"/>
     </row>
-    <row r="301" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A301" s="4">
+        <v>298</v>
+      </c>
       <c r="B301" s="1" t="s">
         <v>859</v>
       </c>
       <c r="C301" s="1" t="s">
         <v>847</v>
       </c>
+      <c r="F301" s="1" t="s">
+        <v>911</v>
+      </c>
       <c r="G301" s="6"/>
     </row>
-    <row r="302" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A302" s="4">
+        <v>299</v>
+      </c>
       <c r="B302" s="1" t="s">
         <v>860</v>
       </c>
@@ -9376,7 +9492,10 @@
       </c>
       <c r="G302" s="6"/>
     </row>
-    <row r="303" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A303" s="4">
+        <v>300</v>
+      </c>
       <c r="B303" s="1" t="s">
         <v>863</v>
       </c>
@@ -9388,7 +9507,10 @@
       </c>
       <c r="G303" s="6"/>
     </row>
-    <row r="304" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A304" s="4">
+        <v>301</v>
+      </c>
       <c r="B304" s="1" t="s">
         <v>864</v>
       </c>
@@ -9400,7 +9522,10 @@
       </c>
       <c r="G304" s="6"/>
     </row>
-    <row r="305" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A305" s="4">
+        <v>302</v>
+      </c>
       <c r="B305" s="1" t="s">
         <v>865</v>
       </c>
@@ -9412,7 +9537,10 @@
       </c>
       <c r="G305" s="6"/>
     </row>
-    <row r="306" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A306" s="4">
+        <v>303</v>
+      </c>
       <c r="B306" s="1" t="s">
         <v>866</v>
       </c>
@@ -9424,7 +9552,10 @@
       </c>
       <c r="G306" s="6"/>
     </row>
-    <row r="307" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A307" s="4">
+        <v>304</v>
+      </c>
       <c r="B307" s="1" t="s">
         <v>867</v>
       </c>
@@ -9436,7 +9567,10 @@
       </c>
       <c r="G307" s="6"/>
     </row>
-    <row r="308" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A308" s="4">
+        <v>305</v>
+      </c>
       <c r="B308" s="1" t="s">
         <v>876</v>
       </c>
@@ -9448,7 +9582,10 @@
       </c>
       <c r="G308" s="6"/>
     </row>
-    <row r="309" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A309" s="4">
+        <v>306</v>
+      </c>
       <c r="B309" s="1" t="s">
         <v>877</v>
       </c>
@@ -9460,7 +9597,10 @@
       </c>
       <c r="G309" s="6"/>
     </row>
-    <row r="310" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A310" s="4">
+        <v>307</v>
+      </c>
       <c r="B310" s="1" t="s">
         <v>879</v>
       </c>
@@ -9472,7 +9612,10 @@
       </c>
       <c r="G310" s="6"/>
     </row>
-    <row r="311" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A311" s="4">
+        <v>308</v>
+      </c>
       <c r="B311" s="1" t="s">
         <v>890</v>
       </c>
@@ -9484,7 +9627,10 @@
       </c>
       <c r="G311" s="6"/>
     </row>
-    <row r="312" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A312" s="4">
+        <v>309</v>
+      </c>
       <c r="B312" s="1" t="s">
         <v>885</v>
       </c>
@@ -9496,7 +9642,10 @@
       </c>
       <c r="G312" s="6"/>
     </row>
-    <row r="313" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A313" s="4">
+        <v>310</v>
+      </c>
       <c r="B313" s="1" t="s">
         <v>883</v>
       </c>
@@ -9508,7 +9657,10 @@
       </c>
       <c r="G313" s="6"/>
     </row>
-    <row r="314" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A314" s="4">
+        <v>311</v>
+      </c>
       <c r="B314" s="1" t="s">
         <v>886</v>
       </c>
@@ -9520,7 +9672,10 @@
       </c>
       <c r="G314" s="6"/>
     </row>
-    <row r="315" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A315" s="4">
+        <v>312</v>
+      </c>
       <c r="B315" s="1" t="s">
         <v>887</v>
       </c>
@@ -9532,7 +9687,10 @@
       </c>
       <c r="G315" s="6"/>
     </row>
-    <row r="316" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A316" s="4">
+        <v>313</v>
+      </c>
       <c r="B316" s="1" t="s">
         <v>900</v>
       </c>
@@ -9544,7 +9702,10 @@
       </c>
       <c r="G316" s="6"/>
     </row>
-    <row r="317" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A317" s="4">
+        <v>314</v>
+      </c>
       <c r="B317" s="1" t="s">
         <v>902</v>
       </c>
@@ -9556,19 +9717,42 @@
       </c>
       <c r="G317" s="6"/>
     </row>
-    <row r="318" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A318" s="4">
+        <v>315</v>
+      </c>
       <c r="B318" s="1" t="s">
         <v>904</v>
       </c>
       <c r="C318" s="1" t="s">
         <v>905</v>
       </c>
+      <c r="F318" s="1" t="s">
+        <v>614</v>
+      </c>
       <c r="G318" s="6"/>
     </row>
-    <row r="319" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="G319" s="6"/>
-    </row>
-    <row r="320" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A319" s="4">
+        <v>316</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="F319" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="G319" s="6" t="s">
+        <v>910</v>
+      </c>
+      <c r="J319" s="18" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="320" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G320" s="6"/>
     </row>
     <row r="321" spans="7:7" x14ac:dyDescent="0.3">
@@ -12263,7 +12447,7 @@
       <c r="G1217" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:K315">
+  <autoFilter ref="B3:K318" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="B4:K288">
       <sortCondition ref="C3:C288"/>
     </sortState>
@@ -12276,185 +12460,188 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1"/>
-    <hyperlink ref="J5" r:id="rId2"/>
-    <hyperlink ref="J6" r:id="rId3"/>
-    <hyperlink ref="J7" r:id="rId4"/>
-    <hyperlink ref="J8" r:id="rId5"/>
-    <hyperlink ref="J9" r:id="rId6"/>
-    <hyperlink ref="J10" r:id="rId7"/>
-    <hyperlink ref="J11" r:id="rId8"/>
-    <hyperlink ref="J12" r:id="rId9"/>
-    <hyperlink ref="J13" r:id="rId10"/>
-    <hyperlink ref="J14" r:id="rId11"/>
-    <hyperlink ref="J15" r:id="rId12"/>
-    <hyperlink ref="J16" r:id="rId13"/>
-    <hyperlink ref="J17" r:id="rId14"/>
-    <hyperlink ref="J18" r:id="rId15"/>
-    <hyperlink ref="J19" r:id="rId16"/>
-    <hyperlink ref="J20" r:id="rId17"/>
-    <hyperlink ref="J21" r:id="rId18"/>
-    <hyperlink ref="J22" r:id="rId19"/>
-    <hyperlink ref="J23" r:id="rId20"/>
-    <hyperlink ref="J24" r:id="rId21"/>
-    <hyperlink ref="J25" r:id="rId22"/>
-    <hyperlink ref="J26" r:id="rId23"/>
-    <hyperlink ref="J27" r:id="rId24"/>
-    <hyperlink ref="J28" r:id="rId25"/>
-    <hyperlink ref="J29" r:id="rId26"/>
-    <hyperlink ref="J30" r:id="rId27"/>
-    <hyperlink ref="J31" r:id="rId28"/>
-    <hyperlink ref="J32" r:id="rId29"/>
-    <hyperlink ref="J33" r:id="rId30"/>
-    <hyperlink ref="J34" r:id="rId31"/>
-    <hyperlink ref="J35" r:id="rId32"/>
-    <hyperlink ref="J36" r:id="rId33"/>
-    <hyperlink ref="J37" r:id="rId34"/>
-    <hyperlink ref="J38" r:id="rId35"/>
-    <hyperlink ref="J39" r:id="rId36"/>
-    <hyperlink ref="J40" r:id="rId37"/>
-    <hyperlink ref="J41" r:id="rId38"/>
-    <hyperlink ref="J42" r:id="rId39"/>
-    <hyperlink ref="J43" r:id="rId40"/>
-    <hyperlink ref="J44" r:id="rId41"/>
-    <hyperlink ref="J45" r:id="rId42"/>
-    <hyperlink ref="J46" r:id="rId43"/>
-    <hyperlink ref="J47" r:id="rId44"/>
-    <hyperlink ref="J48" r:id="rId45"/>
-    <hyperlink ref="J49" r:id="rId46"/>
-    <hyperlink ref="J50" r:id="rId47"/>
-    <hyperlink ref="J51" r:id="rId48"/>
-    <hyperlink ref="J52" r:id="rId49"/>
-    <hyperlink ref="J53" r:id="rId50"/>
-    <hyperlink ref="J54" r:id="rId51"/>
-    <hyperlink ref="J55" r:id="rId52"/>
-    <hyperlink ref="J56" r:id="rId53"/>
-    <hyperlink ref="J57" r:id="rId54"/>
-    <hyperlink ref="J58" r:id="rId55"/>
-    <hyperlink ref="J59" r:id="rId56"/>
-    <hyperlink ref="J60" r:id="rId57"/>
-    <hyperlink ref="J61" r:id="rId58"/>
-    <hyperlink ref="J62" r:id="rId59"/>
-    <hyperlink ref="J63" r:id="rId60"/>
-    <hyperlink ref="J65" r:id="rId61"/>
-    <hyperlink ref="J72" r:id="rId62"/>
-    <hyperlink ref="J73" r:id="rId63"/>
-    <hyperlink ref="J74" r:id="rId64"/>
-    <hyperlink ref="J75" r:id="rId65"/>
-    <hyperlink ref="J76" r:id="rId66"/>
-    <hyperlink ref="J77" r:id="rId67"/>
-    <hyperlink ref="J78" r:id="rId68"/>
-    <hyperlink ref="J79" r:id="rId69"/>
-    <hyperlink ref="J80" r:id="rId70"/>
-    <hyperlink ref="J81" r:id="rId71"/>
-    <hyperlink ref="J82" r:id="rId72"/>
-    <hyperlink ref="J83" r:id="rId73"/>
-    <hyperlink ref="J85" r:id="rId74"/>
-    <hyperlink ref="J86" r:id="rId75"/>
-    <hyperlink ref="J87" r:id="rId76"/>
-    <hyperlink ref="J88" r:id="rId77"/>
-    <hyperlink ref="J93" r:id="rId78"/>
-    <hyperlink ref="J94" r:id="rId79"/>
-    <hyperlink ref="J116" r:id="rId80"/>
-    <hyperlink ref="J84" r:id="rId81"/>
-    <hyperlink ref="J98" r:id="rId82"/>
-    <hyperlink ref="J99" r:id="rId83"/>
-    <hyperlink ref="J250" r:id="rId84"/>
-    <hyperlink ref="J121" r:id="rId85"/>
-    <hyperlink ref="J89" r:id="rId86"/>
-    <hyperlink ref="J90" r:id="rId87"/>
-    <hyperlink ref="J102" r:id="rId88"/>
-    <hyperlink ref="J100" r:id="rId89"/>
-    <hyperlink ref="J103" r:id="rId90"/>
-    <hyperlink ref="J104" r:id="rId91"/>
-    <hyperlink ref="J105" r:id="rId92"/>
-    <hyperlink ref="J106" r:id="rId93"/>
-    <hyperlink ref="J109" r:id="rId94"/>
-    <hyperlink ref="J110" r:id="rId95"/>
-    <hyperlink ref="J111" r:id="rId96"/>
-    <hyperlink ref="J112" r:id="rId97"/>
-    <hyperlink ref="J113" r:id="rId98"/>
-    <hyperlink ref="J114" r:id="rId99"/>
-    <hyperlink ref="J115" r:id="rId100"/>
-    <hyperlink ref="J91" r:id="rId101"/>
-    <hyperlink ref="J92" r:id="rId102"/>
-    <hyperlink ref="J96" r:id="rId103"/>
-    <hyperlink ref="J97" r:id="rId104"/>
-    <hyperlink ref="J120" r:id="rId105"/>
-    <hyperlink ref="J119" r:id="rId106"/>
-    <hyperlink ref="J118" r:id="rId107"/>
-    <hyperlink ref="J117" r:id="rId108"/>
-    <hyperlink ref="J123" r:id="rId109"/>
-    <hyperlink ref="J124" r:id="rId110"/>
-    <hyperlink ref="J205" r:id="rId111"/>
-    <hyperlink ref="J206" r:id="rId112"/>
-    <hyperlink ref="J207" r:id="rId113"/>
-    <hyperlink ref="J208" r:id="rId114"/>
-    <hyperlink ref="J209" r:id="rId115"/>
-    <hyperlink ref="J210" r:id="rId116"/>
-    <hyperlink ref="J211" r:id="rId117"/>
-    <hyperlink ref="J212" r:id="rId118"/>
-    <hyperlink ref="J213" r:id="rId119"/>
-    <hyperlink ref="J214" r:id="rId120"/>
-    <hyperlink ref="J215" r:id="rId121"/>
-    <hyperlink ref="J216" r:id="rId122"/>
-    <hyperlink ref="J217" r:id="rId123"/>
-    <hyperlink ref="J219" r:id="rId124"/>
-    <hyperlink ref="J223" r:id="rId125"/>
-    <hyperlink ref="J222" r:id="rId126"/>
-    <hyperlink ref="J230" r:id="rId127"/>
-    <hyperlink ref="J231" r:id="rId128"/>
-    <hyperlink ref="J232" r:id="rId129"/>
-    <hyperlink ref="J235" r:id="rId130"/>
-    <hyperlink ref="J237" r:id="rId131"/>
-    <hyperlink ref="J241" r:id="rId132"/>
-    <hyperlink ref="J242" r:id="rId133"/>
-    <hyperlink ref="J243" r:id="rId134"/>
-    <hyperlink ref="J245" r:id="rId135"/>
-    <hyperlink ref="J125" r:id="rId136"/>
-    <hyperlink ref="J220" r:id="rId137"/>
-    <hyperlink ref="J126" r:id="rId138"/>
-    <hyperlink ref="J127" r:id="rId139"/>
-    <hyperlink ref="J132" r:id="rId140"/>
-    <hyperlink ref="J131" r:id="rId141"/>
-    <hyperlink ref="J128" r:id="rId142"/>
-    <hyperlink ref="J129" r:id="rId143"/>
-    <hyperlink ref="J133" r:id="rId144"/>
-    <hyperlink ref="J134" r:id="rId145"/>
-    <hyperlink ref="J171" r:id="rId146"/>
-    <hyperlink ref="J172" r:id="rId147"/>
-    <hyperlink ref="J173" r:id="rId148"/>
-    <hyperlink ref="J174" r:id="rId149"/>
-    <hyperlink ref="J175" r:id="rId150"/>
-    <hyperlink ref="J177" r:id="rId151"/>
-    <hyperlink ref="J176" r:id="rId152"/>
-    <hyperlink ref="J178" r:id="rId153"/>
-    <hyperlink ref="J182" r:id="rId154"/>
-    <hyperlink ref="J253" r:id="rId155"/>
-    <hyperlink ref="J251" r:id="rId156"/>
-    <hyperlink ref="J254" r:id="rId157"/>
-    <hyperlink ref="J187" r:id="rId158"/>
-    <hyperlink ref="J188" r:id="rId159"/>
-    <hyperlink ref="J189" r:id="rId160"/>
-    <hyperlink ref="J190" r:id="rId161"/>
-    <hyperlink ref="J191" r:id="rId162"/>
-    <hyperlink ref="J192" r:id="rId163"/>
-    <hyperlink ref="J200" r:id="rId164"/>
-    <hyperlink ref="J193" r:id="rId165"/>
-    <hyperlink ref="J263" r:id="rId166"/>
-    <hyperlink ref="J274" r:id="rId167"/>
-    <hyperlink ref="J275" r:id="rId168"/>
-    <hyperlink ref="J276" r:id="rId169"/>
-    <hyperlink ref="J273" r:id="rId170"/>
-    <hyperlink ref="J18:J23" r:id="rId171" display="FILE"/>
-    <hyperlink ref="J64" r:id="rId172"/>
-    <hyperlink ref="J226" r:id="rId173"/>
-    <hyperlink ref="J228" r:id="rId174"/>
-    <hyperlink ref="J227" r:id="rId175"/>
-    <hyperlink ref="J252" r:id="rId176"/>
-    <hyperlink ref="J204" r:id="rId177"/>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="J6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="J7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="J8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="J9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="J11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="J15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="J17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="J18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="J19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="J20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="J21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="J22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="J23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="J24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="J25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="J26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="J27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="J28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="J29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="J30" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="J31" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="J32" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="J33" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="J34" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="J35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="J36" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="J37" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="J38" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="J39" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="J40" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="J41" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="J42" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="J43" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="J44" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="J45" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="J46" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="J47" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="J48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="J49" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="J50" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="J51" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="J52" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="J53" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="J54" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="J55" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="J56" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="J57" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="J58" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="J59" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="J60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="J61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="J62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="J63" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="J65" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="J72" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="J73" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="J74" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="J75" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="J76" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="J77" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="J78" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="J79" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="J80" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="J81" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="J82" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="J83" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="J85" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="J86" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="J87" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="J88" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="J93" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="J94" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="J116" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="J84" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="J98" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="J99" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="J250" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="J121" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="J89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="J90" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="J102" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="J100" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="J103" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="J104" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="J105" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="J106" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="J109" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="J110" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="J111" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="J112" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="J113" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="J114" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="J115" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="J91" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="J92" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="J96" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="J97" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="J120" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="J119" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="J118" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="J117" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="J123" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="J124" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="J205" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="J206" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="J207" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="J208" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="J209" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="J210" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="J211" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="J212" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="J213" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="J214" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="J215" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="J216" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="J217" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="J219" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="J223" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="J222" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="J230" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="J231" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="J232" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="J235" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="J237" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="J241" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="J242" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="J243" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="J245" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="J125" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="J220" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="J126" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="J127" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="J132" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="J131" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="J128" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="J129" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="J133" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="J134" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="J171" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="J172" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="J173" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="J174" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="J175" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="J177" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="J176" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="J178" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="J182" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="J253" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="J251" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="J254" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="J187" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="J188" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="J189" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="J190" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="J191" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="J192" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="J200" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="J193" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="J263" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="J274" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="J275" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="J276" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="J273" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="J18:J23" r:id="rId171" display="FILE" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="J64" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="J226" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="J228" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="J227" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="J252" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="J204" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="J319" r:id="rId178" xr:uid="{F51F953B-90B6-4940-8D01-A3C9DCD79896}"/>
+    <hyperlink ref="J291" r:id="rId179" xr:uid="{BF7EC704-C084-41E4-8380-3E181DA952E4}"/>
+    <hyperlink ref="J292" r:id="rId180" xr:uid="{50A825A8-1C03-4E64-967E-5D4632584B92}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId178"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId181"/>
 </worksheet>
 </file>
</xml_diff>